<commit_message>
Modified TOF sensor pins
</commit_message>
<xml_diff>
--- a/PIC24_pins.xlsx
+++ b/PIC24_pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Landon\Documents\University of Akron\SDP\autocoffee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6622A1-C3EA-49FC-B458-268DD38D3FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3185E3C4-38EE-474F-8328-0E858EEB8501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24390" yWindow="1920" windowWidth="26265" windowHeight="17730" xr2:uid="{9F69A8B9-D59C-46E1-AAB6-6584CC9B384F}"/>
+    <workbookView xWindow="29040" yWindow="1665" windowWidth="26265" windowHeight="17730" xr2:uid="{9F69A8B9-D59C-46E1-AAB6-6584CC9B384F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="197">
   <si>
     <t>Pin</t>
   </si>
@@ -550,9 +550,6 @@
     <t>TOF2_CE</t>
   </si>
   <si>
-    <t>TOF Sensor 2 Chip Enable</t>
-  </si>
-  <si>
     <t>TOF Sensor 1 Chip Enable</t>
   </si>
   <si>
@@ -562,9 +559,6 @@
     <t>TOF3_CE</t>
   </si>
   <si>
-    <t>TOF Sensor 3 Chip Enable</t>
-  </si>
-  <si>
     <t>Device</t>
   </si>
   <si>
@@ -605,9 +599,6 @@
   </si>
   <si>
     <t>TOF3_GPIO1</t>
-  </si>
-  <si>
-    <t>TOF Sensor 4 Chip Enable</t>
   </si>
   <si>
     <t>TOF4_CE</t>
@@ -1067,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6DB57F5-D47B-4A55-97C3-2C08F13C4EA9}">
   <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,7 +1083,7 @@
         <v>147</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1397,7 +1388,7 @@
         <v>169</v>
       </c>
       <c r="D27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1408,10 +1399,7 @@
         <v>53</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="D28" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1422,10 +1410,7 @@
         <v>54</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="D29" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1436,10 +1421,7 @@
         <v>55</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="D30" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1488,7 +1470,7 @@
         <v>56</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1499,7 +1481,7 @@
         <v>57</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1510,7 +1492,7 @@
         <v>58</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1521,7 +1503,7 @@
         <v>59</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1831,10 +1813,10 @@
         <v>26</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D61" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2045,10 +2027,10 @@
         <v>8</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D77" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2059,10 +2041,10 @@
         <v>9</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D78" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2094,10 +2076,10 @@
         <v>95</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E81" s="6"/>
     </row>
@@ -2109,7 +2091,7 @@
         <v>89</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E82" s="6"/>
     </row>
@@ -2121,7 +2103,7 @@
         <v>90</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E83" s="6"/>
     </row>
@@ -2133,7 +2115,7 @@
         <v>66</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D84" t="s">
         <v>160</v>
@@ -2148,7 +2130,7 @@
         <v>67</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D85" t="s">
         <v>160</v>
@@ -2163,7 +2145,7 @@
         <v>68</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D86" t="s">
         <v>160</v>
@@ -2196,13 +2178,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2210,10 +2192,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2221,10 +2203,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2232,13 +2214,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" t="s">
         <v>183</v>
-      </c>
-      <c r="D4" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2246,13 +2228,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D5" t="s">
         <v>183</v>
-      </c>
-      <c r="D5" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2260,13 +2242,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D6" t="s">
         <v>183</v>
-      </c>
-      <c r="D6" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added proximity sensor pins
</commit_message>
<xml_diff>
--- a/PIC24_pins.xlsx
+++ b/PIC24_pins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Landon\Documents\University of Akron\SDP\autocoffee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3185E3C4-38EE-474F-8328-0E858EEB8501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C9E166-CE1B-4976-A8F8-98EFE1A363C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29040" yWindow="1665" windowWidth="26265" windowHeight="17730" xr2:uid="{9F69A8B9-D59C-46E1-AAB6-6584CC9B384F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9F69A8B9-D59C-46E1-AAB6-6584CC9B384F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="201">
   <si>
     <t>Pin</t>
   </si>
@@ -626,6 +626,18 @@
   </si>
   <si>
     <t>LIMIT</t>
+  </si>
+  <si>
+    <t>PROX1</t>
+  </si>
+  <si>
+    <t>PROX2</t>
+  </si>
+  <si>
+    <t>PROX4</t>
+  </si>
+  <si>
+    <t>PROX3</t>
   </si>
 </sst>
 </file>
@@ -1058,18 +1070,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6DB57F5-D47B-4A55-97C3-2C08F13C4EA9}">
   <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1086,7 +1098,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1095,7 +1107,7 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>3</v>
       </c>
@@ -1107,7 +1119,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>4</v>
       </c>
@@ -1119,7 +1131,7 @@
       </c>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>5</v>
       </c>
@@ -1128,7 +1140,7 @@
       </c>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>6</v>
       </c>
@@ -1142,7 +1154,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>7</v>
       </c>
@@ -1156,7 +1168,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>8</v>
       </c>
@@ -1164,7 +1176,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>9</v>
       </c>
@@ -1172,7 +1184,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>10</v>
       </c>
@@ -1187,7 +1199,7 @@
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>11</v>
       </c>
@@ -1202,7 +1214,7 @@
       </c>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>12</v>
       </c>
@@ -1217,7 +1229,7 @@
       </c>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>14</v>
       </c>
@@ -1232,7 +1244,7 @@
       </c>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>17</v>
       </c>
@@ -1246,7 +1258,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>18</v>
       </c>
@@ -1255,7 +1267,7 @@
       </c>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>19</v>
       </c>
@@ -1264,7 +1276,7 @@
       </c>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>20</v>
       </c>
@@ -1273,7 +1285,7 @@
       </c>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>21</v>
       </c>
@@ -1282,7 +1294,7 @@
       </c>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>22</v>
       </c>
@@ -1290,7 +1302,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>23</v>
       </c>
@@ -1305,7 +1317,7 @@
       </c>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>24</v>
       </c>
@@ -1313,7 +1325,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>25</v>
       </c>
@@ -1321,7 +1333,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>26</v>
       </c>
@@ -1335,7 +1347,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>27</v>
       </c>
@@ -1349,7 +1361,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>28</v>
       </c>
@@ -1363,7 +1375,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>29</v>
       </c>
@@ -1377,7 +1389,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>32</v>
       </c>
@@ -1391,7 +1403,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>33</v>
       </c>
@@ -1402,7 +1414,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>34</v>
       </c>
@@ -1413,7 +1425,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>35</v>
       </c>
@@ -1424,7 +1436,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>38</v>
       </c>
@@ -1432,7 +1444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>39</v>
       </c>
@@ -1447,7 +1459,7 @@
       </c>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>40</v>
       </c>
@@ -1462,7 +1474,7 @@
       </c>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>41</v>
       </c>
@@ -1473,7 +1485,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>42</v>
       </c>
@@ -1484,7 +1496,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>43</v>
       </c>
@@ -1495,7 +1507,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>44</v>
       </c>
@@ -1506,7 +1518,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>47</v>
       </c>
@@ -1521,7 +1533,7 @@
       </c>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>48</v>
       </c>
@@ -1536,7 +1548,7 @@
       </c>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>49</v>
       </c>
@@ -1551,7 +1563,7 @@
       </c>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>50</v>
       </c>
@@ -1566,7 +1578,7 @@
       </c>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>51</v>
       </c>
@@ -1581,7 +1593,7 @@
       </c>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>52</v>
       </c>
@@ -1596,7 +1608,7 @@
       </c>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>53</v>
       </c>
@@ -1611,7 +1623,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>54</v>
       </c>
@@ -1626,7 +1638,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>55</v>
       </c>
@@ -1641,7 +1653,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>56</v>
       </c>
@@ -1656,7 +1668,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>57</v>
       </c>
@@ -1671,7 +1683,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>58</v>
       </c>
@@ -1686,7 +1698,7 @@
       </c>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>59</v>
       </c>
@@ -1701,7 +1713,7 @@
       </c>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>60</v>
       </c>
@@ -1709,7 +1721,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>61</v>
       </c>
@@ -1717,7 +1729,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>63</v>
       </c>
@@ -1731,7 +1743,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>64</v>
       </c>
@@ -1745,7 +1757,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>66</v>
       </c>
@@ -1754,7 +1766,7 @@
       </c>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>67</v>
       </c>
@@ -1763,7 +1775,7 @@
       </c>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>68</v>
       </c>
@@ -1778,7 +1790,7 @@
       </c>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>69</v>
       </c>
@@ -1787,7 +1799,7 @@
       </c>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>70</v>
       </c>
@@ -1796,7 +1808,7 @@
       </c>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>71</v>
       </c>
@@ -1805,7 +1817,7 @@
       </c>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>72</v>
       </c>
@@ -1819,7 +1831,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>73</v>
       </c>
@@ -1833,7 +1845,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>74</v>
       </c>
@@ -1847,7 +1859,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>76</v>
       </c>
@@ -1861,7 +1873,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>77</v>
       </c>
@@ -1875,7 +1887,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>78</v>
       </c>
@@ -1889,7 +1901,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>79</v>
       </c>
@@ -1903,7 +1915,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>80</v>
       </c>
@@ -1917,7 +1929,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>81</v>
       </c>
@@ -1931,7 +1943,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>82</v>
       </c>
@@ -1945,7 +1957,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>83</v>
       </c>
@@ -1959,7 +1971,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>84</v>
       </c>
@@ -1973,7 +1985,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>87</v>
       </c>
@@ -1987,7 +1999,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>88</v>
       </c>
@@ -2001,25 +2013,31 @@
         <v>167</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>89</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="C75" s="5" t="s">
+        <v>199</v>
+      </c>
       <c r="E75" s="6"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>90</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>81</v>
       </c>
+      <c r="C76" s="5" t="s">
+        <v>200</v>
+      </c>
       <c r="E76" s="6"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>91</v>
       </c>
@@ -2033,7 +2051,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>92</v>
       </c>
@@ -2047,31 +2065,37 @@
         <v>191</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>93</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="C79" s="5" t="s">
+        <v>198</v>
+      </c>
       <c r="D79" t="s">
         <v>160</v>
       </c>
       <c r="E79" s="6"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>94</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="C80" s="5" t="s">
+        <v>197</v>
+      </c>
       <c r="D80" t="s">
         <v>160</v>
       </c>
       <c r="E80" s="6"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>95</v>
       </c>
@@ -2083,7 +2107,7 @@
       </c>
       <c r="E81" s="6"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>96</v>
       </c>
@@ -2095,7 +2119,7 @@
       </c>
       <c r="E82" s="6"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>97</v>
       </c>
@@ -2107,7 +2131,7 @@
       </c>
       <c r="E83" s="6"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>98</v>
       </c>
@@ -2122,7 +2146,7 @@
       </c>
       <c r="E84" s="6"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>99</v>
       </c>
@@ -2137,7 +2161,7 @@
       </c>
       <c r="E85" s="6"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>100</v>
       </c>
@@ -2170,13 +2194,13 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>175</v>
       </c>
@@ -2187,7 +2211,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2198,7 +2222,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -2209,7 +2233,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -2223,7 +2247,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -2237,7 +2261,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -2251,47 +2275,47 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>

</xml_diff>